<commit_message>
Excel parser;multiple annotations for article
</commit_message>
<xml_diff>
--- a/Documents/Excel example.xlsx
+++ b/Documents/Excel example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://letsaskq-my.sharepoint.com/personal/stephaan_cloet_letsaskq_com/Documents/Documents/Quinz use cases/Consortium agreements/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c578159010f04de8/Projects/LegalContract/word-contract-assistant/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CBD5E942-86F9-418F-84BC-0EDB995A715C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="8_{CBD5E942-86F9-418F-84BC-0EDB995A715C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{925E891C-F9C1-416F-B350-6AF44A51B1BB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{D4E67FDF-EE43-4ECD-B6C3-0BE62C4F55F0}"/>
+    <workbookView xWindow="2355" yWindow="1305" windowWidth="20940" windowHeight="11790" xr2:uid="{D4E67FDF-EE43-4ECD-B6C3-0BE62C4F55F0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,33 +36,33 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
-  <si>
-    <t>Article 1 - Accounts</t>
-  </si>
-  <si>
-    <t>Article 2 - Content Enrollment and Lifetime Access</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Article 5 - Udemy’s Rights to Content You Post</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>Udemy should not have the right to use user's content in any way</t>
   </si>
   <si>
-    <t>Article 8.4 Payment and billing</t>
-  </si>
-  <si>
     <t>Users from the EU should be able to request a refund anytime during a 14 day period</t>
   </si>
   <si>
-    <t>Article 9.3 Limitation of liability</t>
-  </si>
-  <si>
     <t>Udemy should also be liable for indirect damages and the limit should be uncapped</t>
+  </si>
+  <si>
+    <t>Article</t>
+  </si>
+  <si>
+    <t>Annotation</t>
+  </si>
+  <si>
+    <t>5. Udemy’s Rights to Content You Post</t>
+  </si>
+  <si>
+    <t>9.3 Limitation of liability</t>
+  </si>
+  <si>
+    <t>8.4 Payments and billing</t>
+  </si>
+  <si>
+    <t>Subscription plan can only be changed by user</t>
   </si>
 </sst>
 </file>
@@ -115,6 +115,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -434,64 +438,56 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF9E8D82-C676-45FB-B7ED-0823BABE15CE}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="41.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47" customWidth="1"/>
+    <col min="2" max="2" width="77.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>